<commit_message>
mean nb adults ERFS
</commit_message>
<xml_diff>
--- a/code/quotas.xlsx
+++ b/code/quotas.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="54">
   <si>
     <t>rural</t>
   </si>
@@ -145,6 +145,48 @@
   </si>
   <si>
     <t>education</t>
+  </si>
+  <si>
+    <t>sources:</t>
+  </si>
+  <si>
+    <t>CSP</t>
+  </si>
+  <si>
+    <t>région</t>
+  </si>
+  <si>
+    <t>taille agglo</t>
+  </si>
+  <si>
+    <t>taille agglo bis</t>
+  </si>
+  <si>
+    <t>sexe</t>
+  </si>
+  <si>
+    <t>diplôme</t>
+  </si>
+  <si>
+    <t>https://www.insee.fr/fr/statistiques/2381478</t>
+  </si>
+  <si>
+    <t>https://www.insee.fr/fr/statistiques/1893198</t>
+  </si>
+  <si>
+    <t>own calculation</t>
+  </si>
+  <si>
+    <t>https://www.insee.fr/fr/statistiques/1280970</t>
+  </si>
+  <si>
+    <t>https://www.insee.fr/fr/statistiques/1892088?sommaire=1912926</t>
+  </si>
+  <si>
+    <t>https://www.insee.fr/fr/statistiques/2381474</t>
+  </si>
+  <si>
+    <t>https://www.insee.fr/fr/statistiques/3568823?sommaire=3568833&amp;geo=METRO-1</t>
   </si>
 </sst>
 </file>
@@ -221,7 +263,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -253,6 +295,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -535,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL3"/>
+  <dimension ref="A1:AL10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="A1:AH3"/>
+      <selection activeCell="H10" sqref="A6:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,18 +916,121 @@
       <c r="AK3" s="1"/>
       <c r="AL3" s="1"/>
     </row>
+    <row r="5" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:38" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2">
+        <v>2017</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2019</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2013</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2007</v>
+      </c>
+      <c r="F8" s="2">
+        <v>2019</v>
+      </c>
+      <c r="G8" s="2">
+        <v>2019</v>
+      </c>
+      <c r="H8" s="2">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1"/>
+    <hyperlink ref="C7" r:id="rId2"/>
+    <hyperlink ref="E7" r:id="rId3"/>
+    <hyperlink ref="F7" r:id="rId4"/>
+    <hyperlink ref="G7" r:id="rId5"/>
+    <hyperlink ref="H7" r:id="rId6"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:E23"/>
+      <selection activeCell="A26" sqref="A26:H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1388,7 +1539,110 @@
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
     </row>
+    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="2">
+        <v>2017</v>
+      </c>
+      <c r="C28" s="2">
+        <v>2019</v>
+      </c>
+      <c r="D28" s="2">
+        <v>2013</v>
+      </c>
+      <c r="E28" s="2">
+        <v>2007</v>
+      </c>
+      <c r="F28" s="2">
+        <v>2019</v>
+      </c>
+      <c r="G28" s="2">
+        <v>2019</v>
+      </c>
+      <c r="H28" s="2">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B27" r:id="rId1"/>
+    <hyperlink ref="C27" r:id="rId2"/>
+    <hyperlink ref="E27" r:id="rId3"/>
+    <hyperlink ref="F27" r:id="rId4"/>
+    <hyperlink ref="G27" r:id="rId5"/>
+    <hyperlink ref="H27" r:id="rId6"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>